<commit_message>
n°paquete deleted and format in secado added
</commit_message>
<xml_diff>
--- a/bin/Debug/StockFenólicos.xlsx
+++ b/bin/Debug/StockFenólicos.xlsx
@@ -37,43 +37,7 @@
     <x:t>Premium</x:t>
   </x:si>
   <x:si>
-    <x:t>10 cm</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Normal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20 cm</x:t>
-  </x:si>
-  <x:si>
-    <x:t>normal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>100cm</x:t>
-  </x:si>
-  <x:si>
-    <x:t>premium</x:t>
-  </x:si>
-  <x:si>
-    <x:t>medio pelo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9cm</x:t>
-  </x:si>
-  <x:si>
-    <x:t>100</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Caca</x:t>
-  </x:si>
-  <x:si>
-    <x:t>100mm</x:t>
-  </x:si>
-  <x:si>
-    <x:t>God</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pedo</x:t>
+    <x:t>10cm</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -167,7 +131,7 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="7">
+  <x:cellXfs count="6">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -190,10 +154,6 @@
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -491,35 +451,31 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F23"/>
+  <x:dimension ref="A1:D12"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="16.710625" style="0" customWidth="1"/>
-    <x:col min="2" max="3" width="17.710625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="20.710625" style="0" customWidth="1"/>
-    <x:col min="5" max="6" width="25.710625" style="0" customWidth="1"/>
+    <x:col min="1" max="2" width="20.710625" style="0" customWidth="1"/>
+    <x:col min="3" max="4" width="25.710625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="9" spans="1:6">
+    <x:row r="9" spans="1:4">
       <x:c r="B9" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="C9" s="2"/>
     </x:row>
-    <x:row r="10" spans="1:6">
+    <x:row r="10" spans="1:4">
       <x:c r="A10" s="3" t="s">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B10" s="4"/>
       <x:c r="C10" s="4"/>
       <x:c r="D10" s="4"/>
-      <x:c r="E10" s="2"/>
-      <x:c r="F10" s="2"/>
     </x:row>
-    <x:row r="11" spans="1:6">
+    <x:row r="11" spans="1:4">
       <x:c r="A11" s="5" t="s">
         <x:v>2</x:v>
       </x:c>
@@ -532,159 +488,19 @@
       <x:c r="D11" s="5" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="E11" s="2"/>
-      <x:c r="F11" s="2"/>
     </x:row>
-    <x:row r="12" spans="1:6">
-      <x:c r="A12" s="6"/>
-      <x:c r="B12" s="6"/>
-      <x:c r="C12" s="6"/>
-      <x:c r="D12" s="6"/>
-    </x:row>
-    <x:row r="13" spans="1:6">
-      <x:c r="A13" s="6"/>
-      <x:c r="B13" s="6"/>
-      <x:c r="C13" s="6"/>
-      <x:c r="D13" s="6"/>
-    </x:row>
-    <x:row r="14" spans="1:6">
-      <x:c r="A14" s="5" t="s">
+    <x:row r="12" spans="1:4">
+      <x:c r="A12" s="5" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="B14" s="5" t="s">
+      <x:c r="B12" s="5" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="C14" s="5">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="D14" s="5">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:6">
-      <x:c r="A15" s="5" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B15" s="5" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C15" s="5">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="D15" s="5">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:6">
-      <x:c r="A16" s="5" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B16" s="5" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C16" s="5">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="D16" s="5">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:6">
-      <x:c r="A17" s="5" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B17" s="5" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C17" s="5">
-        <x:v>231</x:v>
-      </x:c>
-      <x:c r="D17" s="5">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:6">
-      <x:c r="A18" s="5" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="B18" s="5" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="C18" s="5">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="D18" s="5">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:6">
-      <x:c r="A19" s="5" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="B19" s="5" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="C19" s="5">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="D19" s="5">
-        <x:v>905</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:6">
-      <x:c r="A20" s="5" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B20" s="5" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C20" s="5">
-        <x:v>1090</x:v>
-      </x:c>
-      <x:c r="D20" s="5">
-        <x:v>19</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:6">
-      <x:c r="A21" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B21" s="5" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C21" s="5">
+      <x:c r="C12" s="5">
         <x:v>100</x:v>
       </x:c>
-      <x:c r="D21" s="5">
-        <x:v>910</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:6">
-      <x:c r="A22" s="5" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="B22" s="5" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C22" s="5">
-        <x:v>1000</x:v>
-      </x:c>
-      <x:c r="D22" s="5">
-        <x:v>1000000</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:6">
-      <x:c r="A23" s="5" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="B23" s="5" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C23" s="5">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="D23" s="5">
-        <x:v>100</x:v>
+      <x:c r="D12" s="5">
+        <x:v>1095</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>